<commit_message>
Revert "Revert "update something""
</commit_message>
<xml_diff>
--- a/Diet Balance Game/Assets/Textures/Food/FoodData.xlsx
+++ b/Diet Balance Game/Assets/Textures/Food/FoodData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E240AB38-0BAF-493B-93AA-ED7AAF054849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29704B92-BB24-47AB-A10D-A6C7BC2266AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,95 +20,306 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Energy</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Carb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Lipid</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Protein</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Vitamin</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Mineral</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>crepe</t>
-  </si>
-  <si>
-    <t>ramen</t>
-  </si>
-  <si>
-    <t>salad</t>
-  </si>
-  <si>
-    <t>zaru_udon</t>
-  </si>
-  <si>
-    <t>zaru_soba</t>
-  </si>
-  <si>
-    <t>egg</t>
-  </si>
-  <si>
-    <t>hamburger</t>
-  </si>
-  <si>
-    <t>orange_juice</t>
-  </si>
-  <si>
-    <t>beef_bowl</t>
-  </si>
-  <si>
-    <t>yakiniku</t>
-  </si>
-  <si>
-    <t>tempura</t>
-  </si>
-  <si>
-    <t>pork_soup</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>energy[kcal]</t>
+  </si>
+  <si>
+    <t>protein[g]</t>
+  </si>
+  <si>
+    <t>Lipids[g]</t>
+  </si>
+  <si>
+    <t>carbohydrates[g]</t>
+  </si>
+  <si>
+    <t>vitamin[mg]</t>
+  </si>
+  <si>
+    <t>mineral[mg]</t>
+  </si>
+  <si>
+    <t>crepes</t>
+  </si>
+  <si>
+    <t>Chunky_ramen</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Zaru_udon</t>
+  </si>
+  <si>
+    <t>Zaru_soba</t>
+  </si>
+  <si>
+    <t>Boiled eggs</t>
+  </si>
+  <si>
+    <t>Humburger</t>
+  </si>
+  <si>
     <t>pizza</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fruit juices</t>
+  </si>
+  <si>
+    <t>Gyudon</t>
+  </si>
+  <si>
+    <t>Grilled meat</t>
+  </si>
+  <si>
+    <t>Tempra</t>
+  </si>
+  <si>
+    <t>Tonjiru</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>Carbonara</t>
+  </si>
+  <si>
+    <t>Curry_rice</t>
+  </si>
+  <si>
+    <t>Grilled chicken</t>
+  </si>
+  <si>
+    <t>Grilled fish</t>
+  </si>
+  <si>
+    <t>Grilled rice</t>
+  </si>
+  <si>
+    <t>Gyoza</t>
+  </si>
+  <si>
+    <t>Hamburger steak</t>
+  </si>
+  <si>
+    <t>Kimchi</t>
+  </si>
+  <si>
+    <t>Mandarin Orange</t>
+  </si>
+  <si>
+    <t>Neapolitan</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>Sakura mochi</t>
+  </si>
+  <si>
+    <t>Shortcake</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>steak</t>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>クレープ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>醤油ラーメン</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>野菜サラダ</t>
+    <rPh sb="0" eb="2">
+      <t>ヤサイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ざるうどん</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ざるそば</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>たまご</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ハンバーガー</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ピザ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>オレンジジュース</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>牛丼</t>
+    <rPh sb="0" eb="2">
+      <t>ギュウドン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>和牛モモ肉(250g)</t>
+    <rPh sb="0" eb="2">
+      <t>ワギュウ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ニク</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>天ぷらの盛り合わせ</t>
+    <rPh sb="0" eb="1">
+      <t>テン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ア</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>豚汁</t>
+    <rPh sb="0" eb="2">
+      <t>トンジル</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ビール</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>カルボナーラ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>カレーライス</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>焼き鳥</t>
+    <rPh sb="0" eb="1">
+      <t>ヤ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>トリ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ほっけの塩焼き</t>
+    <rPh sb="4" eb="6">
+      <t>シオヤ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>チャーハン</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>餃子(200g)</t>
+    <rPh sb="0" eb="2">
+      <t>ギョウザ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ハンバーグ(150g)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>キムチ(150g)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>みかん</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ナポリタン</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ご飯</t>
+    <rPh sb="1" eb="2">
+      <t>ハン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>桜餅</t>
+    <rPh sb="0" eb="2">
+      <t>サクラモチ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ショートケーキ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>豆腐とわかめの味噌汁</t>
+    <rPh sb="0" eb="2">
+      <t>トウフ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>ミソシル</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ステーキ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>いちご</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Yu Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="等线"/>
+      <name val="Yu Gothic"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -119,6 +330,13 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,12 +359,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,46 +645,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="9" max="9" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.5">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>566</v>
@@ -486,10 +708,13 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5">
+      <c r="I2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>470</v>
@@ -512,10 +737,13 @@
       <c r="H3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -538,10 +766,13 @@
       <c r="H4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>289</v>
@@ -564,10 +795,13 @@
       <c r="H5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>366</v>
@@ -590,10 +824,13 @@
       <c r="H6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>91</v>
@@ -616,10 +853,13 @@
       <c r="H7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>422</v>
@@ -642,10 +882,13 @@
       <c r="H8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>872</v>
@@ -668,10 +911,13 @@
       <c r="H9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>214</v>
@@ -694,10 +940,13 @@
       <c r="H10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>771</v>
@@ -720,10 +969,13 @@
       <c r="H11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>615</v>
@@ -746,10 +998,13 @@
       <c r="H12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>167</v>
@@ -772,10 +1027,13 @@
       <c r="H13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>121</v>
@@ -797,6 +1055,502 @@
       </c>
       <c r="H14">
         <v>13</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>142</v>
+      </c>
+      <c r="C15">
+        <v>1.06</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>10.97</v>
+      </c>
+      <c r="F15">
+        <v>3.3883200000000002</v>
+      </c>
+      <c r="G15">
+        <v>219.52353999999997</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>779</v>
+      </c>
+      <c r="C16">
+        <v>26.32</v>
+      </c>
+      <c r="D16">
+        <v>39.49</v>
+      </c>
+      <c r="E16">
+        <v>72.38</v>
+      </c>
+      <c r="F16">
+        <v>13.841670000000001</v>
+      </c>
+      <c r="G16">
+        <v>2341.4540699999993</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>859</v>
+      </c>
+      <c r="C17">
+        <v>21.03</v>
+      </c>
+      <c r="D17">
+        <v>26.51</v>
+      </c>
+      <c r="E17">
+        <v>129.16999999999999</v>
+      </c>
+      <c r="F17">
+        <v>38.012070000000001</v>
+      </c>
+      <c r="G17">
+        <v>2750.7221099999997</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>99</v>
+      </c>
+      <c r="C18">
+        <v>7.53</v>
+      </c>
+      <c r="D18">
+        <v>6.3</v>
+      </c>
+      <c r="E18">
+        <v>1.73</v>
+      </c>
+      <c r="F18">
+        <v>4.7419799999999999</v>
+      </c>
+      <c r="G18">
+        <v>422.43953999999991</v>
+      </c>
+      <c r="H18">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>461</v>
+      </c>
+      <c r="C19">
+        <v>69.209999999999994</v>
+      </c>
+      <c r="D19">
+        <v>17.61</v>
+      </c>
+      <c r="E19">
+        <v>0.4</v>
+      </c>
+      <c r="F19">
+        <v>27.390770000000003</v>
+      </c>
+      <c r="G19">
+        <v>4436.0700799999986</v>
+      </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>708</v>
+      </c>
+      <c r="C20">
+        <v>18.97</v>
+      </c>
+      <c r="D20">
+        <v>24.05</v>
+      </c>
+      <c r="E20">
+        <v>97.64</v>
+      </c>
+      <c r="F20">
+        <v>13.3857</v>
+      </c>
+      <c r="G20">
+        <v>2213.0943299999999</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>394</v>
+      </c>
+      <c r="C21">
+        <v>14.2</v>
+      </c>
+      <c r="D21">
+        <v>16.2</v>
+      </c>
+      <c r="E21">
+        <v>47.6</v>
+      </c>
+      <c r="F21">
+        <v>14.406000000000001</v>
+      </c>
+      <c r="G21">
+        <v>1582</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>335</v>
+      </c>
+      <c r="C22">
+        <v>19.95</v>
+      </c>
+      <c r="D22">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E22">
+        <v>18.45</v>
+      </c>
+      <c r="F22">
+        <v>4.9664000000000001</v>
+      </c>
+      <c r="G22">
+        <v>1334.7495000000001</v>
+      </c>
+      <c r="H22">
+        <v>21</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>69</v>
+      </c>
+      <c r="C23">
+        <v>4.2</v>
+      </c>
+      <c r="D23">
+        <v>0.45</v>
+      </c>
+      <c r="E23">
+        <v>11.85</v>
+      </c>
+      <c r="F23">
+        <v>39.399000000000001</v>
+      </c>
+      <c r="G23">
+        <v>1996.7</v>
+      </c>
+      <c r="H23">
+        <v>22</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>0.53</v>
+      </c>
+      <c r="D24">
+        <v>0.08</v>
+      </c>
+      <c r="E24">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F24">
+        <v>25.665800000000001</v>
+      </c>
+      <c r="G24">
+        <v>143.47000000000003</v>
+      </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>590</v>
+      </c>
+      <c r="C25">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="D25">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="E25">
+        <v>78.72</v>
+      </c>
+      <c r="F25">
+        <v>24.562750000000001</v>
+      </c>
+      <c r="G25">
+        <v>2314.4266600000005</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>269</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>0.48</v>
+      </c>
+      <c r="E26">
+        <v>59.36</v>
+      </c>
+      <c r="F26">
+        <v>0.80560000000000009</v>
+      </c>
+      <c r="G26">
+        <v>120.28959999999999</v>
+      </c>
+      <c r="H26">
+        <v>25</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>96</v>
+      </c>
+      <c r="C27">
+        <v>1.8</v>
+      </c>
+      <c r="D27">
+        <v>0.16</v>
+      </c>
+      <c r="E27">
+        <v>21.72</v>
+      </c>
+      <c r="F27">
+        <v>0.1016</v>
+      </c>
+      <c r="G27">
+        <v>56.86999999999999</v>
+      </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>366</v>
+      </c>
+      <c r="C28">
+        <v>4.59</v>
+      </c>
+      <c r="D28">
+        <v>25.3</v>
+      </c>
+      <c r="E28">
+        <v>29.05</v>
+      </c>
+      <c r="F28">
+        <v>11.154590000000001</v>
+      </c>
+      <c r="G28">
+        <v>270.66522999999995</v>
+      </c>
+      <c r="H28">
+        <v>27</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>56</v>
+      </c>
+      <c r="C29">
+        <v>3.98</v>
+      </c>
+      <c r="D29">
+        <v>1.69</v>
+      </c>
+      <c r="E29">
+        <v>6.34</v>
+      </c>
+      <c r="F29">
+        <v>1.9807800000000002</v>
+      </c>
+      <c r="G29">
+        <v>899.95059000000015</v>
+      </c>
+      <c r="H29">
+        <v>28</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>355</v>
+      </c>
+      <c r="C30">
+        <v>18</v>
+      </c>
+      <c r="D30">
+        <v>28.51</v>
+      </c>
+      <c r="E30">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F30">
+        <v>7.3321899999999998</v>
+      </c>
+      <c r="G30">
+        <v>1018.27075</v>
+      </c>
+      <c r="H30">
+        <v>29</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D31">
+        <v>0.06</v>
+      </c>
+      <c r="E31">
+        <v>5.19</v>
+      </c>
+      <c r="F31">
+        <v>38.606000000000002</v>
+      </c>
+      <c r="G31">
+        <v>141.36610000000002</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>